<commit_message>
SI570 added to CVO list
</commit_message>
<xml_diff>
--- a/DCO_PCB/cmp.xlsx
+++ b/DCO_PCB/cmp.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boti&amp;Ima\Desktop\Work\BG2016\Etapa2018\prototype\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boti&amp;Ima\Desktop\Work\BG2016\Etapa2018\NAPOSIP\DCO_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="7515" activeTab="3"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="7515" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Prescaler" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="162">
   <si>
     <t>Nr biti</t>
   </si>
@@ -506,6 +506,18 @@
   </si>
   <si>
     <t>NB7N017M</t>
+  </si>
+  <si>
+    <t>https://www.silabs.com/documents/public/data-sheets/si570.pdf</t>
+  </si>
+  <si>
+    <t>1.8, 2.5, or 3.3 V supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10 MHz to 1400 MHz</t>
+  </si>
+  <si>
+    <t>Si570</t>
   </si>
 </sst>
 </file>
@@ -3492,7 +3504,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3588,10 +3600,18 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
+      <c r="A8" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>158</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>